<commit_message>
Added interrupts and some scheduler stuff
</commit_message>
<xml_diff>
--- a/pin assignments.xlsx
+++ b/pin assignments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Pins from L to R</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>PHA1</t>
+  </si>
+  <si>
+    <t>Pulse Measurement</t>
+  </si>
+  <si>
+    <t>PF0 / PWM0</t>
   </si>
 </sst>
 </file>
@@ -468,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,6 +671,14 @@
       </c>
       <c r="D14" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lab 2 Release 1.0
Comments added. Removed communication from major cycle schedule.
</commit_message>
<xml_diff>
--- a/pin assignments.xlsx
+++ b/pin assignments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Pins from L to R</t>
   </si>
@@ -151,6 +151,24 @@
   </si>
   <si>
     <t>PHA1</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>PWM0</t>
+  </si>
+  <si>
+    <t>Pulse input</t>
+  </si>
+  <si>
+    <t>Timing output</t>
+  </si>
+  <si>
+    <t>PF3</t>
+  </si>
+  <si>
+    <t>LED0</t>
   </si>
 </sst>
 </file>
@@ -468,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +628,9 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
@@ -624,6 +645,9 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
@@ -638,6 +662,9 @@
       <c r="B12" t="s">
         <v>15</v>
       </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
@@ -655,6 +682,9 @@
       <c r="B13" t="s">
         <v>17</v>
       </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
@@ -663,8 +693,30 @@
       <c r="A14" t="s">
         <v>22</v>
       </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
       <c r="D14" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>